<commit_message>
Spaghetti and MER completed
</commit_message>
<xml_diff>
--- a/Assignment-2/targetting_calculations.xlsx
+++ b/Assignment-2/targetting_calculations.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PTA" sheetId="1" r:id="rId1"/>
     <sheet name="Spaghetti" sheetId="2" r:id="rId2"/>
+    <sheet name="MER" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>sum(FCphot)</t>
   </si>
@@ -66,6 +67,21 @@
   </si>
   <si>
     <t xml:space="preserve">U </t>
+  </si>
+  <si>
+    <t>Area Target</t>
+  </si>
+  <si>
+    <t>Cost Hex</t>
+  </si>
+  <si>
+    <t>Utility Costs</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Annualization factor</t>
   </si>
 </sst>
 </file>
@@ -717,20 +733,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1">
-        <v>1E-3</v>
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <v>0.25</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -787,7 +813,7 @@
       </c>
       <c r="H3">
         <f>B3/B$1/G3</f>
-        <v>419.28582712547592</v>
+        <v>0.41928582712547591</v>
       </c>
       <c r="J3">
         <f xml:space="preserve"> LN((D3-E3)/(C3-F3))</f>
@@ -825,6 +851,14 @@
       <c r="F4">
         <v>162</v>
       </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G13" si="0">((D4-E4)-(C4-F4))/LN((D4-E4)/(C4-F4))</f>
+        <v>12.984255368000671</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H13" si="1">B4/B$1/G4</f>
+        <v>4.8520302639196169</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -845,6 +879,14 @@
       <c r="F5">
         <v>141</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>11.570821021688559</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.8702216514660099</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -865,6 +907,14 @@
       <c r="F6">
         <v>141</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>11.570821021688559</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0.98186636701965524</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -885,11 +935,22 @@
       <c r="F7">
         <v>130</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>17.300699854438779</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>12.138237283280828</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
+      <c r="B8">
+        <v>47.05</v>
+      </c>
       <c r="C8">
         <v>144.59</v>
       </c>
@@ -901,12 +962,23 @@
       </c>
       <c r="F8">
         <v>130</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>17.300699854438779</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>2.7195431627541096</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
+      <c r="B9">
+        <v>139.95099999999999</v>
+      </c>
       <c r="C9">
         <v>144.59</v>
       </c>
@@ -918,16 +990,425 @@
       </c>
       <c r="F9">
         <v>130</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>17.300699854438779</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>8.0893259334877872</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
+      <c r="B10">
+        <v>26.85</v>
+      </c>
+      <c r="C10">
+        <v>80.328000000000003</v>
+      </c>
+      <c r="D10">
+        <v>67.540000000000006</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>28.05963735210441</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0.95689048518605713</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>80.328000000000003</v>
+      </c>
+      <c r="D11">
+        <v>67.540000000000006</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>28.05963735210441</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>2.7797935882499982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>7</v>
+      </c>
+      <c r="B12">
+        <v>57.893999999999998</v>
+      </c>
+      <c r="C12">
+        <v>67.540000000000006</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>30.846340467771046</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.8768514877960631</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>110.16</v>
+      </c>
+      <c r="C13">
+        <v>67.540000000000006</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>30.846340467771046</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>3.5712502141087903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <f xml:space="preserve"> SUM(H4:H13)</f>
+        <v>39.836010437268925</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <f xml:space="preserve"> 11*(40000+500*H14/11)</f>
+        <v>459918.00521863444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <f xml:space="preserve"> 120*B3+10*(B12+B13)</f>
+        <v>8160.54</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <f>0.25*H15+H16</f>
+        <v>123140.0413046586</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3">
+        <v>162</v>
+      </c>
+      <c r="F3">
+        <v>180</v>
+      </c>
+      <c r="G3">
+        <f>((D3-E3)-(C3-F3))/LN((D3-E3)/(C3-F3))</f>
+        <v>128.79042530536074</v>
+      </c>
+      <c r="H3">
+        <f>B3/B$1/G3</f>
+        <v>0.41928582712547591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>63</v>
+      </c>
+      <c r="C4">
+        <v>180</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="E4">
+        <v>141</v>
+      </c>
+      <c r="F4">
+        <v>162</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G8" si="0">((D4-E4)-(C4-F4))/LN((D4-E4)/(C4-F4))</f>
+        <v>12.984255368000671</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H8" si="1">B4/B$1/G4</f>
+        <v>4.8520302639196169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>231</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>130</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>14.426950408889635</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>16.011699870934734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>243</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6">
+        <v>81.998999999999995</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>141</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>14.543970817033021</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>16.707954317084649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <v>81.998999999999995</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>130</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>33.489545522916721</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.86594187968766112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>168</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>81.998999999999995</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>90.939811938735573</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.8473757138752214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9">
+        <f>SUM(H3:H8)</f>
+        <v>40.704287872627361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10">
+        <f xml:space="preserve"> 6*(40000+H9/6)</f>
+        <v>240040.70428787262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <f xml:space="preserve"> 120*B3+10*B8</f>
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <f xml:space="preserve"> E$1*H10+H11</f>
+        <v>68170.176071968162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>